<commit_message>
Fix category filtering bug, improve terminology
+ Better logging
</commit_message>
<xml_diff>
--- a/original/PersRep_Data Pseud.xlsx
+++ b/original/PersRep_Data Pseud.xlsx
@@ -30,100 +30,100 @@
     <t xml:space="preserve">course</t>
   </si>
   <si>
-    <t xml:space="preserve">num/eb/my_score/Week2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/eb/total_score/Week2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/eb/my_score/Week7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/eb/total_score/Week7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/vb/my_score/Week2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/vb/total_score/Week2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/vb/my_score/Week7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/vb/total_score/Week7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/my_score/Time point 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/total_score/Time point 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/my_score/Time point 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/total_score/Time point 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/my_score/Time point 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/total_score/Time point 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/my_score/Time point 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ae/total_score/Time point 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/my_score/Time point 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/total_score/Time point 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/my_score/Time point 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/total_score/Time point 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/my_score/Time point 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/total_score/Time point 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/my_score/Time point 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/be/total_score/Time point 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/my_score/Time point 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/total_score/Time point 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/my_score/Time point 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/total_score/Time point 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/my_score/Time point 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/total_score/Time point 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/my_score/Time point 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num/ce/total_score/Time point 4</t>
+    <t xml:space="preserve">num/eb/My score/Week2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/eb/Total score/Week2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/eb/My score/Week7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/eb/Total score/Week7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/vb/My score/Week2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/vb/Total score/Week2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/vb/My score/Week7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/vb/Total score/Week7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/My score/Time point 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/Total score/Time point 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/My score/Time point 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/Total score/Time point 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/My score/Time point 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/Total score/Time point 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/My score/Time point 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ae/Total score/Time point 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/My score/Time point 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/Total score/Time point 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/My score/Time point 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/Total score/Time point 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/My score/Time point 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/Total score/Time point 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/My score/Time point 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/be/Total score/Time point 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/My score/Time point 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/Total score/Time point 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/My score/Time point 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/Total score/Time point 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/My score/Time point 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/Total score/Time point 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/My score/Time point 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num/ce/Total score/Time point 4</t>
   </si>
   <si>
     <t xml:space="preserve">S001</t>
@@ -992,7 +992,7 @@
   <dimension ref="A1:AI109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4999,7 +4999,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="C1:AH1 A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5057,7 +5057,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="C1:AH1 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>